<commit_message>
Metropolis-Hasitings and Markov Chains
</commit_message>
<xml_diff>
--- a/I&E 352/Marketing_Metrics/Marketing_Metrics.xlsx
+++ b/I&E 352/Marketing_Metrics/Marketing_Metrics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaanyadav/Desktop/Duke Courses/I&amp;E 352/Marketing_Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15025ABA-1275-D84F-8182-FCE9AF5D2E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEE067E-FCD5-9A4A-A391-B87CBFB4769A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="700" windowWidth="26740" windowHeight="16260" xr2:uid="{093E48A8-0986-C645-B331-F19C3229CF3D}"/>
+    <workbookView xWindow="140" yWindow="700" windowWidth="26900" windowHeight="16860" xr2:uid="{093E48A8-0986-C645-B331-F19C3229CF3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>RFC Gross Sales Revenue to Retailers</t>
   </si>
@@ -113,9 +113,6 @@
     <t>these are redone due to increased sale</t>
   </si>
   <si>
-    <t>unchangerd because no indication of increase COGS in question - otherwise would increase</t>
-  </si>
-  <si>
     <t>Data - Question 3</t>
   </si>
   <si>
@@ -132,6 +129,18 @@
   </si>
   <si>
     <t>Increase in $ sales needed</t>
+  </si>
+  <si>
+    <t>changes because more goods therefore more COGs</t>
+  </si>
+  <si>
+    <t>600,000 + 20*0.15*units sold</t>
+  </si>
+  <si>
+    <t>900,000 = 9*goods sold - 600,000</t>
+  </si>
+  <si>
+    <t>166,666 need to be sold</t>
   </si>
 </sst>
 </file>
@@ -140,7 +149,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -192,18 +201,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -539,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D705DF54-A9AE-634F-9CDF-D67608D73C7B}">
-  <dimension ref="C3:K49"/>
+  <dimension ref="C3:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,8 +594,8 @@
         <v>13</v>
       </c>
       <c r="D6" s="5">
-        <f>I4-I8-I5</f>
-        <v>1500000</v>
+        <f>I4-I8</f>
+        <v>1800000</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>2</v>
@@ -601,8 +609,8 @@
         <v>15</v>
       </c>
       <c r="D7" s="6">
-        <f>(D6/I6)*100</f>
-        <v>55.555555555555557</v>
+        <f>D6/I4 * 100</f>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -613,8 +621,8 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <f>I9+I10+I13</f>
-        <v>600000</v>
+        <f>I9+I10+I13+I5</f>
+        <v>900000</v>
       </c>
       <c r="H8" t="s">
         <v>3</v>
@@ -629,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="5">
-        <f>I6-I8-D8</f>
+        <f>I4-I8-D8</f>
         <v>900000</v>
       </c>
       <c r="H9" t="s">
@@ -644,8 +652,8 @@
         <v>18</v>
       </c>
       <c r="D10">
-        <f>(D9/I6)*100</f>
-        <v>33.333333333333329</v>
+        <f>D9/I4 * 100</f>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -662,8 +670,8 @@
         <v>19</v>
       </c>
       <c r="D11">
-        <f>(D9/D8)*100</f>
-        <v>150</v>
+        <f>D9/D8 *100</f>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -738,7 +746,7 @@
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="7"/>
       <c r="H22" s="4" t="s">
@@ -757,18 +765,18 @@
         <v>14</v>
       </c>
       <c r="D24" s="5">
-        <f>I25+I26+I29</f>
-        <v>700000</v>
+        <f>I25+I26+I29+I21</f>
+        <v>1160000</v>
       </c>
       <c r="H24" t="s">
         <v>3</v>
       </c>
       <c r="I24" s="3">
-        <f>I8</f>
-        <v>1200000</v>
+        <f>I8 + I8*(8/15)</f>
+        <v>1840000</v>
       </c>
       <c r="J24" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.2">
@@ -776,8 +784,8 @@
         <v>17</v>
       </c>
       <c r="D25" s="5">
-        <f>I22-I24-D24</f>
-        <v>2240000</v>
+        <f>I20-I24-D24</f>
+        <v>1600000</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -794,8 +802,8 @@
         <v>18</v>
       </c>
       <c r="D26">
-        <f>(D25/I22)*100</f>
-        <v>54.106280193236714</v>
+        <f>(D25/I20)*100</f>
+        <v>34.782608695652172</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -813,7 +821,7 @@
       </c>
       <c r="D27">
         <f>(D25/D24)*100</f>
-        <v>320</v>
+        <v>137.93103448275863</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -866,12 +874,12 @@
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="H35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C36" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="7"/>
       <c r="H36" t="s">
@@ -895,8 +903,8 @@
         <v>13</v>
       </c>
       <c r="D38" s="5">
-        <f>I36-I40-I37</f>
-        <v>1350000</v>
+        <f>I36-I40</f>
+        <v>1800000</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>2</v>
@@ -911,8 +919,8 @@
         <v>15</v>
       </c>
       <c r="D39" s="6">
-        <f>(D38/I38)*100</f>
-        <v>52.941176470588239</v>
+        <f>(D38/I36)*100</f>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
@@ -920,8 +928,8 @@
         <v>14</v>
       </c>
       <c r="D40" s="5">
-        <f>I41+I42+I45</f>
-        <v>600000</v>
+        <f>I41+I42+I45+I37</f>
+        <v>1050000</v>
       </c>
       <c r="H40" t="s">
         <v>3</v>
@@ -935,7 +943,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="5">
-        <f>I38-I40-D40</f>
+        <f>I36-I40-D40</f>
         <v>750000</v>
       </c>
       <c r="H41" t="s">
@@ -950,8 +958,11 @@
         <v>18</v>
       </c>
       <c r="D42">
-        <f>(D41/I38)*100</f>
-        <v>29.411764705882355</v>
+        <f>(D41/I36)*100</f>
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
       </c>
       <c r="H42" t="s">
         <v>5</v>
@@ -966,7 +977,10 @@
       </c>
       <c r="D43">
         <f>(D41/D40)*100</f>
-        <v>125</v>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
       </c>
       <c r="H43" t="s">
         <v>6</v>
@@ -984,11 +998,9 @@
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
       <c r="H45" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1010,7 @@
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47">
         <v>15</v>
@@ -1017,6 +1029,7 @@
       </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D48" s="5"/>
       <c r="H48" t="s">
         <v>11</v>
       </c>
@@ -1024,14 +1037,27 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="E49" t="s">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54">
+        <v>11.11</v>
+      </c>
+      <c r="E54" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>